<commit_message>
Started OO design and implementation
</commit_message>
<xml_diff>
--- a/res/ecm2414_cover_page_and_devlog.xlsx
+++ b/res/ecm2414_cover_page_and_devlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/ac1198_exeter_ac_uk/Documents/Documents/ECM2414/Continuous Assessment/cards/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABDACC10483C799C54165BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F55B1E27-F1C5-47AC-8213-CD99DDF59A95}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_F25DC773A252ABDACC10483C799C54165BDE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{405EDDA9-B695-4718-90EF-74EDDC4C7FE8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Student ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Weight</t>
   </si>
@@ -49,6 +46,33 @@
   </si>
   <si>
     <t>ECM2414 Cover Page</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Observer</t>
+  </si>
+  <si>
+    <t>Joey</t>
+  </si>
+  <si>
+    <t>Joey Signature</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Alexander Signature</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Joey Role</t>
+  </si>
+  <si>
+    <t>Alexander Role</t>
   </si>
 </sst>
 </file>
@@ -131,11 +155,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -146,42 +167,61 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:H21"/>
+  <dimension ref="C3:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,152 +516,196 @@
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="25.44140625" customWidth="1"/>
     <col min="7" max="7" width="27.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="19.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C8" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C10" s="6">
+        <v>44865</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E10" s="18">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="H10" s="21">
         <v>710022765</v>
       </c>
-      <c r="F5" s="4">
+      <c r="I10" s="14">
         <v>710033804</v>
       </c>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="D6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C8" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="7" t="s">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C11" s="6"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C12" s="6"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C13" s="6"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C14" s="6"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="19"/>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C15" s="6"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C16" s="6"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="7">
-        <v>710022765</v>
-      </c>
-      <c r="G9" s="7">
-        <v>710033804</v>
-      </c>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="8"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10"/>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C11" s="8"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="10"/>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C12" s="8"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C13" s="8"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="10"/>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C14" s="8"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C15" s="8"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C16" s="8"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="10"/>
-      <c r="H16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C17" s="8"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="15"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="16"/>
-    </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C19" s="16"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="16"/>
-    </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C20" s="16"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="16"/>
-    </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C21" s="16"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="16"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C17" s="6"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C18" s="13"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C19" s="14"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C21" s="14"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Updated cover sheet, assembled cards.jar
</commit_message>
<xml_diff>
--- a/res/ecm2414_cover_page_and_devlog.xlsx
+++ b/res/ecm2414_cover_page_and_devlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/ac1198_exeter_ac_uk/Documents/Documents/ECM2414/cards/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/ac1198_exeter_ac_uk/Documents/Documents/ECM2414/Continuous Assessment/cards/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_2C016E1713B6237AFF5F824038940A10FB1FE673" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06356922-7DEA-4FAF-B676-E2089CB32EBB}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_2C016E1713B6237AFF5F824038940A10FB1FE673" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8B55959-77F3-493E-B320-DEFE26DC678B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>ECM2414 Cover Page</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Driver</t>
+  </si>
+  <si>
+    <t>22/22/2022</t>
   </si>
 </sst>
 </file>
@@ -236,10 +239,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -454,8 +453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="107" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -673,11 +672,21 @@
       </c>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="10"/>
+      <c r="C16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E16" s="8">
+        <v>9.375E-2</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="H16" s="15">
         <v>710022765</v>
       </c>
@@ -704,12 +713,8 @@
       <c r="E18" s="12"/>
       <c r="F18" s="15"/>
       <c r="G18" s="12"/>
-      <c r="H18" s="15">
-        <v>710022765</v>
-      </c>
-      <c r="I18" s="12">
-        <v>710033804</v>
-      </c>
+      <c r="H18" s="15"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C19" s="12"/>
@@ -717,12 +722,8 @@
       <c r="E19" s="12"/>
       <c r="F19" s="15"/>
       <c r="G19" s="12"/>
-      <c r="H19" s="15">
-        <v>710022765</v>
-      </c>
-      <c r="I19" s="12">
-        <v>710033804</v>
-      </c>
+      <c r="H19" s="15"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C20" s="12"/>
@@ -730,12 +731,8 @@
       <c r="E20" s="12"/>
       <c r="F20" s="15"/>
       <c r="G20" s="12"/>
-      <c r="H20" s="15">
-        <v>710022765</v>
-      </c>
-      <c r="I20" s="12">
-        <v>710033804</v>
-      </c>
+      <c r="H20" s="15"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C21" s="12"/>

</xml_diff>